<commit_message>
display toeic test, create countdown timer
</commit_message>
<xml_diff>
--- a/back-end/uploads/TEST1/Questions.xlsx
+++ b/back-end/uploads/TEST1/Questions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="1063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="1062">
   <si>
     <t>section</t>
   </si>
@@ -2192,9 +2192,6 @@
   </si>
   <si>
     <t>146 (A)</t>
-  </si>
-  <si>
-    <t>.</t>
   </si>
   <si>
     <t>Where is the information most likely found?</t>
@@ -3603,8 +3600,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="G141" sqref="G141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3631,7 +3628,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -7682,7 +7679,7 @@
         <v>463</v>
       </c>
       <c r="B132" s="23" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C132" s="23">
         <v>131</v>
@@ -7715,7 +7712,7 @@
         <v>463</v>
       </c>
       <c r="B133" s="23" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C133" s="23">
         <v>132</v>
@@ -7748,7 +7745,7 @@
         <v>463</v>
       </c>
       <c r="B134" s="23" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C134" s="23">
         <v>133</v>
@@ -7781,7 +7778,7 @@
         <v>463</v>
       </c>
       <c r="B135" s="23" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="C135" s="23">
         <v>134</v>
@@ -7814,7 +7811,7 @@
         <v>463</v>
       </c>
       <c r="B136" s="23" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="C136" s="23">
         <v>135</v>
@@ -7847,7 +7844,7 @@
         <v>463</v>
       </c>
       <c r="B137" s="23" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="C137" s="23">
         <v>136</v>
@@ -7880,7 +7877,7 @@
         <v>463</v>
       </c>
       <c r="B138" s="23" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="C138" s="23">
         <v>137</v>
@@ -7913,7 +7910,7 @@
         <v>463</v>
       </c>
       <c r="B139" s="23" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="C139" s="23">
         <v>138</v>
@@ -7946,7 +7943,7 @@
         <v>463</v>
       </c>
       <c r="B140" s="23" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C140" s="23">
         <v>139</v>
@@ -7979,7 +7976,7 @@
         <v>463</v>
       </c>
       <c r="B141" s="23" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C141" s="23">
         <v>140</v>
@@ -8012,7 +8009,7 @@
         <v>463</v>
       </c>
       <c r="B142" s="23" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C142" s="23">
         <v>141</v>
@@ -8045,7 +8042,7 @@
         <v>463</v>
       </c>
       <c r="B143" s="23" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C143" s="23">
         <v>142</v>
@@ -8078,7 +8075,7 @@
         <v>463</v>
       </c>
       <c r="B144" s="23" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C144" s="23">
         <v>143</v>
@@ -8111,7 +8108,7 @@
         <v>463</v>
       </c>
       <c r="B145" s="23" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C145" s="23">
         <v>144</v>
@@ -8144,7 +8141,7 @@
         <v>463</v>
       </c>
       <c r="B146" s="23" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C146" s="23">
         <v>145</v>
@@ -8177,7 +8174,7 @@
         <v>463</v>
       </c>
       <c r="B147" s="23" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="C147" s="23">
         <v>146</v>
@@ -8210,35 +8207,33 @@
         <v>463</v>
       </c>
       <c r="B148" s="27" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="C148" s="27">
         <v>147</v>
       </c>
-      <c r="D148" s="27" t="s">
-        <v>723</v>
-      </c>
+      <c r="D148" s="27"/>
       <c r="E148" s="28"/>
       <c r="F148" s="27">
         <v>7</v>
       </c>
       <c r="G148" s="29" t="s">
+        <v>723</v>
+      </c>
+      <c r="H148" s="27" t="s">
         <v>724</v>
       </c>
-      <c r="H148" s="27" t="s">
+      <c r="I148" s="27" t="s">
         <v>725</v>
       </c>
-      <c r="I148" s="27" t="s">
+      <c r="J148" s="27" t="s">
         <v>726</v>
       </c>
-      <c r="J148" s="27" t="s">
+      <c r="K148" s="27" t="s">
         <v>727</v>
       </c>
-      <c r="K148" s="27" t="s">
+      <c r="L148" s="29" t="s">
         <v>728</v>
-      </c>
-      <c r="L148" s="29" t="s">
-        <v>729</v>
       </c>
       <c r="M148" s="28"/>
     </row>
@@ -8247,7 +8242,7 @@
         <v>463</v>
       </c>
       <c r="B149" s="27" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="C149" s="27">
         <v>148</v>
@@ -8258,22 +8253,22 @@
         <v>7</v>
       </c>
       <c r="G149" s="29" t="s">
+        <v>729</v>
+      </c>
+      <c r="H149" s="27" t="s">
         <v>730</v>
       </c>
-      <c r="H149" s="27" t="s">
+      <c r="I149" s="27" t="s">
         <v>731</v>
       </c>
-      <c r="I149" s="27" t="s">
+      <c r="J149" s="27" t="s">
         <v>732</v>
       </c>
-      <c r="J149" s="27" t="s">
+      <c r="K149" s="27" t="s">
         <v>733</v>
       </c>
-      <c r="K149" s="27" t="s">
+      <c r="L149" s="29" t="s">
         <v>734</v>
-      </c>
-      <c r="L149" s="29" t="s">
-        <v>735</v>
       </c>
       <c r="M149" s="28"/>
     </row>
@@ -8282,7 +8277,7 @@
         <v>463</v>
       </c>
       <c r="B150" s="27" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="C150" s="27">
         <v>149</v>
@@ -8293,22 +8288,22 @@
         <v>7</v>
       </c>
       <c r="G150" s="29" t="s">
+        <v>735</v>
+      </c>
+      <c r="H150" s="27" t="s">
         <v>736</v>
       </c>
-      <c r="H150" s="27" t="s">
+      <c r="I150" s="27" t="s">
         <v>737</v>
       </c>
-      <c r="I150" s="27" t="s">
+      <c r="J150" s="27" t="s">
         <v>738</v>
       </c>
-      <c r="J150" s="27" t="s">
+      <c r="K150" s="27" t="s">
         <v>739</v>
       </c>
-      <c r="K150" s="27" t="s">
+      <c r="L150" s="29" t="s">
         <v>740</v>
-      </c>
-      <c r="L150" s="29" t="s">
-        <v>741</v>
       </c>
       <c r="M150" s="28"/>
     </row>
@@ -8317,7 +8312,7 @@
         <v>463</v>
       </c>
       <c r="B151" s="27" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="C151" s="27">
         <v>150</v>
@@ -8328,22 +8323,22 @@
         <v>7</v>
       </c>
       <c r="G151" s="29" t="s">
+        <v>741</v>
+      </c>
+      <c r="H151" s="27" t="s">
         <v>742</v>
       </c>
-      <c r="H151" s="27" t="s">
+      <c r="I151" s="27" t="s">
         <v>743</v>
       </c>
-      <c r="I151" s="27" t="s">
+      <c r="J151" s="27" t="s">
         <v>744</v>
       </c>
-      <c r="J151" s="27" t="s">
+      <c r="K151" s="27" t="s">
         <v>745</v>
       </c>
-      <c r="K151" s="27" t="s">
+      <c r="L151" s="29" t="s">
         <v>746</v>
-      </c>
-      <c r="L151" s="29" t="s">
-        <v>747</v>
       </c>
       <c r="M151" s="28"/>
     </row>
@@ -8352,7 +8347,7 @@
         <v>463</v>
       </c>
       <c r="B152" s="27" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C152" s="27">
         <v>151</v>
@@ -8363,22 +8358,22 @@
         <v>7</v>
       </c>
       <c r="G152" s="29" t="s">
+        <v>747</v>
+      </c>
+      <c r="H152" s="27" t="s">
         <v>748</v>
       </c>
-      <c r="H152" s="27" t="s">
+      <c r="I152" s="27" t="s">
         <v>749</v>
       </c>
-      <c r="I152" s="27" t="s">
+      <c r="J152" s="27" t="s">
         <v>750</v>
       </c>
-      <c r="J152" s="27" t="s">
+      <c r="K152" s="27" t="s">
         <v>751</v>
       </c>
-      <c r="K152" s="27" t="s">
+      <c r="L152" s="29" t="s">
         <v>752</v>
-      </c>
-      <c r="L152" s="29" t="s">
-        <v>753</v>
       </c>
       <c r="M152" s="28"/>
     </row>
@@ -8387,7 +8382,7 @@
         <v>463</v>
       </c>
       <c r="B153" s="27" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C153" s="27">
         <v>152</v>
@@ -8398,22 +8393,22 @@
         <v>7</v>
       </c>
       <c r="G153" s="29" t="s">
+        <v>753</v>
+      </c>
+      <c r="H153" s="27" t="s">
         <v>754</v>
       </c>
-      <c r="H153" s="27" t="s">
+      <c r="I153" s="27" t="s">
         <v>755</v>
       </c>
-      <c r="I153" s="27" t="s">
+      <c r="J153" s="27" t="s">
         <v>756</v>
       </c>
-      <c r="J153" s="27" t="s">
+      <c r="K153" s="27" t="s">
         <v>757</v>
       </c>
-      <c r="K153" s="27" t="s">
+      <c r="L153" s="29" t="s">
         <v>758</v>
-      </c>
-      <c r="L153" s="29" t="s">
-        <v>759</v>
       </c>
       <c r="M153" s="28"/>
     </row>
@@ -8422,7 +8417,7 @@
         <v>463</v>
       </c>
       <c r="B154" s="27" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="C154" s="27">
         <v>153</v>
@@ -8433,22 +8428,22 @@
         <v>7</v>
       </c>
       <c r="G154" s="29" t="s">
+        <v>759</v>
+      </c>
+      <c r="H154" s="27" t="s">
         <v>760</v>
       </c>
-      <c r="H154" s="27" t="s">
+      <c r="I154" s="27" t="s">
         <v>761</v>
       </c>
-      <c r="I154" s="27" t="s">
+      <c r="J154" s="27" t="s">
         <v>762</v>
       </c>
-      <c r="J154" s="27" t="s">
+      <c r="K154" s="27" t="s">
         <v>763</v>
       </c>
-      <c r="K154" s="27" t="s">
+      <c r="L154" s="29" t="s">
         <v>764</v>
-      </c>
-      <c r="L154" s="29" t="s">
-        <v>765</v>
       </c>
       <c r="M154" s="28"/>
     </row>
@@ -8457,7 +8452,7 @@
         <v>463</v>
       </c>
       <c r="B155" s="27" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="C155" s="27">
         <v>154</v>
@@ -8468,22 +8463,22 @@
         <v>7</v>
       </c>
       <c r="G155" s="29" t="s">
+        <v>765</v>
+      </c>
+      <c r="H155" s="27" t="s">
         <v>766</v>
       </c>
-      <c r="H155" s="27" t="s">
+      <c r="I155" s="27" t="s">
         <v>767</v>
       </c>
-      <c r="I155" s="27" t="s">
+      <c r="J155" s="27" t="s">
         <v>768</v>
       </c>
-      <c r="J155" s="27" t="s">
+      <c r="K155" s="27" t="s">
         <v>769</v>
       </c>
-      <c r="K155" s="27" t="s">
+      <c r="L155" s="29" t="s">
         <v>770</v>
-      </c>
-      <c r="L155" s="29" t="s">
-        <v>771</v>
       </c>
       <c r="M155" s="28"/>
     </row>
@@ -8492,7 +8487,7 @@
         <v>463</v>
       </c>
       <c r="B156" s="27" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="C156" s="27">
         <v>155</v>
@@ -8503,22 +8498,22 @@
         <v>7</v>
       </c>
       <c r="G156" s="29" t="s">
+        <v>771</v>
+      </c>
+      <c r="H156" s="27" t="s">
         <v>772</v>
       </c>
-      <c r="H156" s="27" t="s">
+      <c r="I156" s="27" t="s">
         <v>773</v>
       </c>
-      <c r="I156" s="27" t="s">
+      <c r="J156" s="27" t="s">
         <v>774</v>
       </c>
-      <c r="J156" s="27" t="s">
+      <c r="K156" s="27" t="s">
         <v>775</v>
       </c>
-      <c r="K156" s="27" t="s">
+      <c r="L156" s="29" t="s">
         <v>776</v>
-      </c>
-      <c r="L156" s="29" t="s">
-        <v>777</v>
       </c>
       <c r="M156" s="28"/>
     </row>
@@ -8527,7 +8522,7 @@
         <v>463</v>
       </c>
       <c r="B157" s="27" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="C157" s="27">
         <v>156</v>
@@ -8538,22 +8533,22 @@
         <v>7</v>
       </c>
       <c r="G157" s="29" t="s">
+        <v>777</v>
+      </c>
+      <c r="H157" s="27" t="s">
         <v>778</v>
       </c>
-      <c r="H157" s="27" t="s">
+      <c r="I157" s="27" t="s">
         <v>779</v>
       </c>
-      <c r="I157" s="27" t="s">
+      <c r="J157" s="27" t="s">
         <v>780</v>
       </c>
-      <c r="J157" s="27" t="s">
+      <c r="K157" s="27" t="s">
         <v>781</v>
       </c>
-      <c r="K157" s="27" t="s">
+      <c r="L157" s="29" t="s">
         <v>782</v>
-      </c>
-      <c r="L157" s="29" t="s">
-        <v>783</v>
       </c>
       <c r="M157" s="28"/>
     </row>
@@ -8562,7 +8557,7 @@
         <v>463</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="C158" s="27">
         <v>157</v>
@@ -8573,22 +8568,22 @@
         <v>7</v>
       </c>
       <c r="G158" s="29" t="s">
+        <v>783</v>
+      </c>
+      <c r="H158" s="27" t="s">
         <v>784</v>
       </c>
-      <c r="H158" s="27" t="s">
+      <c r="I158" s="27" t="s">
         <v>785</v>
       </c>
-      <c r="I158" s="27" t="s">
+      <c r="J158" s="27" t="s">
         <v>786</v>
       </c>
-      <c r="J158" s="27" t="s">
+      <c r="K158" s="27" t="s">
         <v>787</v>
       </c>
-      <c r="K158" s="27" t="s">
+      <c r="L158" s="29" t="s">
         <v>788</v>
-      </c>
-      <c r="L158" s="29" t="s">
-        <v>789</v>
       </c>
       <c r="M158" s="28"/>
     </row>
@@ -8597,7 +8592,7 @@
         <v>463</v>
       </c>
       <c r="B159" s="27" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="C159" s="27">
         <v>158</v>
@@ -8608,22 +8603,22 @@
         <v>7</v>
       </c>
       <c r="G159" s="29" t="s">
+        <v>789</v>
+      </c>
+      <c r="H159" s="27" t="s">
         <v>790</v>
       </c>
-      <c r="H159" s="27" t="s">
+      <c r="I159" s="27" t="s">
         <v>791</v>
-      </c>
-      <c r="I159" s="27" t="s">
-        <v>792</v>
       </c>
       <c r="J159" s="27" t="s">
         <v>412</v>
       </c>
       <c r="K159" s="27" t="s">
+        <v>792</v>
+      </c>
+      <c r="L159" s="29" t="s">
         <v>793</v>
-      </c>
-      <c r="L159" s="29" t="s">
-        <v>794</v>
       </c>
       <c r="M159" s="28"/>
     </row>
@@ -8632,7 +8627,7 @@
         <v>463</v>
       </c>
       <c r="B160" s="27" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="C160" s="27">
         <v>159</v>
@@ -8643,22 +8638,22 @@
         <v>7</v>
       </c>
       <c r="G160" s="29" t="s">
+        <v>794</v>
+      </c>
+      <c r="H160" s="27" t="s">
         <v>795</v>
       </c>
-      <c r="H160" s="27" t="s">
+      <c r="I160" s="27" t="s">
         <v>796</v>
       </c>
-      <c r="I160" s="27" t="s">
+      <c r="J160" s="27" t="s">
         <v>797</v>
       </c>
-      <c r="J160" s="27" t="s">
+      <c r="K160" s="27" t="s">
         <v>798</v>
       </c>
-      <c r="K160" s="27" t="s">
+      <c r="L160" s="29" t="s">
         <v>799</v>
-      </c>
-      <c r="L160" s="29" t="s">
-        <v>800</v>
       </c>
       <c r="M160" s="28"/>
     </row>
@@ -8667,7 +8662,7 @@
         <v>463</v>
       </c>
       <c r="B161" s="27" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="C161" s="27">
         <v>160</v>
@@ -8678,22 +8673,22 @@
         <v>7</v>
       </c>
       <c r="G161" s="29" t="s">
+        <v>800</v>
+      </c>
+      <c r="H161" s="27" t="s">
         <v>801</v>
       </c>
-      <c r="H161" s="27" t="s">
+      <c r="I161" s="27" t="s">
         <v>802</v>
       </c>
-      <c r="I161" s="27" t="s">
+      <c r="J161" s="27" t="s">
         <v>803</v>
       </c>
-      <c r="J161" s="27" t="s">
+      <c r="K161" s="27" t="s">
         <v>804</v>
       </c>
-      <c r="K161" s="27" t="s">
+      <c r="L161" s="29" t="s">
         <v>805</v>
-      </c>
-      <c r="L161" s="29" t="s">
-        <v>806</v>
       </c>
       <c r="M161" s="28"/>
     </row>
@@ -8702,7 +8697,7 @@
         <v>463</v>
       </c>
       <c r="B162" s="27" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C162" s="27">
         <v>161</v>
@@ -8713,22 +8708,22 @@
         <v>7</v>
       </c>
       <c r="G162" s="29" t="s">
+        <v>806</v>
+      </c>
+      <c r="H162" s="27" t="s">
         <v>807</v>
       </c>
-      <c r="H162" s="27" t="s">
+      <c r="I162" s="27" t="s">
         <v>808</v>
       </c>
-      <c r="I162" s="27" t="s">
+      <c r="J162" s="27" t="s">
         <v>809</v>
       </c>
-      <c r="J162" s="27" t="s">
+      <c r="K162" s="27" t="s">
         <v>810</v>
       </c>
-      <c r="K162" s="27" t="s">
+      <c r="L162" s="29" t="s">
         <v>811</v>
-      </c>
-      <c r="L162" s="29" t="s">
-        <v>812</v>
       </c>
       <c r="M162" s="28"/>
     </row>
@@ -8737,7 +8732,7 @@
         <v>463</v>
       </c>
       <c r="B163" s="27" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C163" s="27">
         <v>162</v>
@@ -8748,22 +8743,22 @@
         <v>7</v>
       </c>
       <c r="G163" s="29" t="s">
+        <v>812</v>
+      </c>
+      <c r="H163" s="27" t="s">
         <v>813</v>
       </c>
-      <c r="H163" s="27" t="s">
+      <c r="I163" s="27" t="s">
         <v>814</v>
       </c>
-      <c r="I163" s="27" t="s">
+      <c r="J163" s="27" t="s">
         <v>815</v>
       </c>
-      <c r="J163" s="27" t="s">
+      <c r="K163" s="27" t="s">
         <v>816</v>
       </c>
-      <c r="K163" s="27" t="s">
+      <c r="L163" s="29" t="s">
         <v>817</v>
-      </c>
-      <c r="L163" s="29" t="s">
-        <v>818</v>
       </c>
       <c r="M163" s="28"/>
     </row>
@@ -8772,7 +8767,7 @@
         <v>463</v>
       </c>
       <c r="B164" s="27" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C164" s="27">
         <v>163</v>
@@ -8783,22 +8778,22 @@
         <v>7</v>
       </c>
       <c r="G164" s="29" t="s">
+        <v>818</v>
+      </c>
+      <c r="H164" s="27" t="s">
         <v>819</v>
       </c>
-      <c r="H164" s="27" t="s">
+      <c r="I164" s="27" t="s">
         <v>820</v>
       </c>
-      <c r="I164" s="27" t="s">
+      <c r="J164" s="27" t="s">
         <v>821</v>
       </c>
-      <c r="J164" s="27" t="s">
+      <c r="K164" s="27" t="s">
         <v>822</v>
       </c>
-      <c r="K164" s="27" t="s">
+      <c r="L164" s="29" t="s">
         <v>823</v>
-      </c>
-      <c r="L164" s="29" t="s">
-        <v>824</v>
       </c>
       <c r="M164" s="28"/>
     </row>
@@ -8807,7 +8802,7 @@
         <v>463</v>
       </c>
       <c r="B165" s="27" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C165" s="27">
         <v>164</v>
@@ -8818,22 +8813,22 @@
         <v>7</v>
       </c>
       <c r="G165" s="29" t="s">
+        <v>824</v>
+      </c>
+      <c r="H165" s="27" t="s">
         <v>825</v>
       </c>
-      <c r="H165" s="27" t="s">
+      <c r="I165" s="27" t="s">
         <v>826</v>
       </c>
-      <c r="I165" s="27" t="s">
+      <c r="J165" s="27" t="s">
         <v>827</v>
       </c>
-      <c r="J165" s="27" t="s">
+      <c r="K165" s="27" t="s">
         <v>828</v>
       </c>
-      <c r="K165" s="27" t="s">
+      <c r="L165" s="29" t="s">
         <v>829</v>
-      </c>
-      <c r="L165" s="29" t="s">
-        <v>830</v>
       </c>
       <c r="M165" s="28"/>
     </row>
@@ -8842,7 +8837,7 @@
         <v>463</v>
       </c>
       <c r="B166" s="27" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="C166" s="27">
         <v>165</v>
@@ -8853,22 +8848,22 @@
         <v>7</v>
       </c>
       <c r="G166" s="29" t="s">
+        <v>830</v>
+      </c>
+      <c r="H166" s="27" t="s">
         <v>831</v>
       </c>
-      <c r="H166" s="27" t="s">
+      <c r="I166" s="27" t="s">
         <v>832</v>
       </c>
-      <c r="I166" s="27" t="s">
+      <c r="J166" s="27" t="s">
         <v>833</v>
       </c>
-      <c r="J166" s="27" t="s">
+      <c r="K166" s="27" t="s">
         <v>834</v>
       </c>
-      <c r="K166" s="27" t="s">
+      <c r="L166" s="29" t="s">
         <v>835</v>
-      </c>
-      <c r="L166" s="29" t="s">
-        <v>836</v>
       </c>
       <c r="M166" s="28"/>
     </row>
@@ -8877,7 +8872,7 @@
         <v>463</v>
       </c>
       <c r="B167" s="27" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="C167" s="27">
         <v>166</v>
@@ -8888,22 +8883,22 @@
         <v>7</v>
       </c>
       <c r="G167" s="29" t="s">
+        <v>836</v>
+      </c>
+      <c r="H167" s="27" t="s">
         <v>837</v>
       </c>
-      <c r="H167" s="27" t="s">
+      <c r="I167" s="27" t="s">
         <v>838</v>
       </c>
-      <c r="I167" s="27" t="s">
+      <c r="J167" s="27" t="s">
         <v>839</v>
       </c>
-      <c r="J167" s="27" t="s">
+      <c r="K167" s="27" t="s">
         <v>840</v>
       </c>
-      <c r="K167" s="27" t="s">
+      <c r="L167" s="29" t="s">
         <v>841</v>
-      </c>
-      <c r="L167" s="29" t="s">
-        <v>842</v>
       </c>
       <c r="M167" s="28"/>
     </row>
@@ -8912,7 +8907,7 @@
         <v>463</v>
       </c>
       <c r="B168" s="27" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="C168" s="27">
         <v>167</v>
@@ -8923,22 +8918,22 @@
         <v>7</v>
       </c>
       <c r="G168" s="29" t="s">
+        <v>842</v>
+      </c>
+      <c r="H168" s="27" t="s">
         <v>843</v>
       </c>
-      <c r="H168" s="27" t="s">
+      <c r="I168" s="27" t="s">
         <v>844</v>
       </c>
-      <c r="I168" s="27" t="s">
+      <c r="J168" s="27" t="s">
         <v>845</v>
       </c>
-      <c r="J168" s="27" t="s">
+      <c r="K168" s="27" t="s">
         <v>846</v>
       </c>
-      <c r="K168" s="27" t="s">
+      <c r="L168" s="29" t="s">
         <v>847</v>
-      </c>
-      <c r="L168" s="29" t="s">
-        <v>848</v>
       </c>
       <c r="M168" s="28"/>
     </row>
@@ -8947,7 +8942,7 @@
         <v>463</v>
       </c>
       <c r="B169" s="27" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="C169" s="27">
         <v>168</v>
@@ -8958,22 +8953,22 @@
         <v>7</v>
       </c>
       <c r="G169" s="29" t="s">
+        <v>848</v>
+      </c>
+      <c r="H169" s="27" t="s">
         <v>849</v>
       </c>
-      <c r="H169" s="27" t="s">
+      <c r="I169" s="27" t="s">
         <v>850</v>
       </c>
-      <c r="I169" s="27" t="s">
+      <c r="J169" s="27" t="s">
         <v>851</v>
       </c>
-      <c r="J169" s="27" t="s">
+      <c r="K169" s="27" t="s">
         <v>852</v>
       </c>
-      <c r="K169" s="27" t="s">
+      <c r="L169" s="29" t="s">
         <v>853</v>
-      </c>
-      <c r="L169" s="29" t="s">
-        <v>854</v>
       </c>
       <c r="M169" s="28"/>
     </row>
@@ -8982,7 +8977,7 @@
         <v>463</v>
       </c>
       <c r="B170" s="27" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="C170" s="27">
         <v>169</v>
@@ -8993,22 +8988,22 @@
         <v>7</v>
       </c>
       <c r="G170" s="29" t="s">
+        <v>854</v>
+      </c>
+      <c r="H170" s="27" t="s">
         <v>855</v>
       </c>
-      <c r="H170" s="27" t="s">
+      <c r="I170" s="27" t="s">
         <v>856</v>
       </c>
-      <c r="I170" s="27" t="s">
+      <c r="J170" s="27" t="s">
         <v>857</v>
       </c>
-      <c r="J170" s="27" t="s">
+      <c r="K170" s="27" t="s">
         <v>858</v>
       </c>
-      <c r="K170" s="27" t="s">
+      <c r="L170" s="29" t="s">
         <v>859</v>
-      </c>
-      <c r="L170" s="29" t="s">
-        <v>860</v>
       </c>
       <c r="M170" s="28"/>
     </row>
@@ -9017,7 +9012,7 @@
         <v>463</v>
       </c>
       <c r="B171" s="27" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="C171" s="27">
         <v>170</v>
@@ -9028,22 +9023,22 @@
         <v>7</v>
       </c>
       <c r="G171" s="29" t="s">
+        <v>860</v>
+      </c>
+      <c r="H171" s="27" t="s">
         <v>861</v>
       </c>
-      <c r="H171" s="27" t="s">
+      <c r="I171" s="27" t="s">
         <v>862</v>
       </c>
-      <c r="I171" s="27" t="s">
+      <c r="J171" s="27" t="s">
         <v>863</v>
       </c>
-      <c r="J171" s="27" t="s">
+      <c r="K171" s="27" t="s">
         <v>864</v>
       </c>
-      <c r="K171" s="27" t="s">
+      <c r="L171" s="29" t="s">
         <v>865</v>
-      </c>
-      <c r="L171" s="29" t="s">
-        <v>866</v>
       </c>
       <c r="M171" s="28"/>
     </row>
@@ -9052,7 +9047,7 @@
         <v>463</v>
       </c>
       <c r="B172" s="27" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="C172" s="27">
         <v>171</v>
@@ -9063,22 +9058,22 @@
         <v>7</v>
       </c>
       <c r="G172" s="29" t="s">
+        <v>866</v>
+      </c>
+      <c r="H172" s="27" t="s">
+        <v>801</v>
+      </c>
+      <c r="I172" s="27" t="s">
+        <v>802</v>
+      </c>
+      <c r="J172" s="27" t="s">
+        <v>803</v>
+      </c>
+      <c r="K172" s="27" t="s">
+        <v>804</v>
+      </c>
+      <c r="L172" s="29" t="s">
         <v>867</v>
-      </c>
-      <c r="H172" s="27" t="s">
-        <v>802</v>
-      </c>
-      <c r="I172" s="27" t="s">
-        <v>803</v>
-      </c>
-      <c r="J172" s="27" t="s">
-        <v>804</v>
-      </c>
-      <c r="K172" s="27" t="s">
-        <v>805</v>
-      </c>
-      <c r="L172" s="29" t="s">
-        <v>868</v>
       </c>
       <c r="M172" s="28"/>
     </row>
@@ -9087,7 +9082,7 @@
         <v>463</v>
       </c>
       <c r="B173" s="27" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C173" s="27">
         <v>172</v>
@@ -9098,22 +9093,22 @@
         <v>7</v>
       </c>
       <c r="G173" s="29" t="s">
+        <v>868</v>
+      </c>
+      <c r="H173" s="27" t="s">
         <v>869</v>
       </c>
-      <c r="H173" s="27" t="s">
+      <c r="I173" s="27" t="s">
         <v>870</v>
       </c>
-      <c r="I173" s="27" t="s">
+      <c r="J173" s="27" t="s">
         <v>871</v>
       </c>
-      <c r="J173" s="27" t="s">
+      <c r="K173" s="27" t="s">
         <v>872</v>
       </c>
-      <c r="K173" s="27" t="s">
+      <c r="L173" s="29" t="s">
         <v>873</v>
-      </c>
-      <c r="L173" s="29" t="s">
-        <v>874</v>
       </c>
       <c r="M173" s="28"/>
     </row>
@@ -9122,7 +9117,7 @@
         <v>463</v>
       </c>
       <c r="B174" s="27" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C174" s="27">
         <v>173</v>
@@ -9133,22 +9128,22 @@
         <v>7</v>
       </c>
       <c r="G174" s="29" t="s">
+        <v>874</v>
+      </c>
+      <c r="H174" s="27" t="s">
         <v>875</v>
       </c>
-      <c r="H174" s="27" t="s">
+      <c r="I174" s="27" t="s">
         <v>876</v>
       </c>
-      <c r="I174" s="27" t="s">
+      <c r="J174" s="27" t="s">
         <v>877</v>
       </c>
-      <c r="J174" s="27" t="s">
+      <c r="K174" s="27" t="s">
         <v>878</v>
       </c>
-      <c r="K174" s="27" t="s">
+      <c r="L174" s="29" t="s">
         <v>879</v>
-      </c>
-      <c r="L174" s="29" t="s">
-        <v>880</v>
       </c>
       <c r="M174" s="28"/>
     </row>
@@ -9157,7 +9152,7 @@
         <v>463</v>
       </c>
       <c r="B175" s="27" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C175" s="27">
         <v>174</v>
@@ -9168,22 +9163,22 @@
         <v>7</v>
       </c>
       <c r="G175" s="29" t="s">
+        <v>880</v>
+      </c>
+      <c r="H175" s="27" t="s">
         <v>881</v>
       </c>
-      <c r="H175" s="27" t="s">
+      <c r="I175" s="27" t="s">
         <v>882</v>
       </c>
-      <c r="I175" s="27" t="s">
+      <c r="J175" s="27" t="s">
         <v>883</v>
       </c>
-      <c r="J175" s="27" t="s">
+      <c r="K175" s="27" t="s">
         <v>884</v>
       </c>
-      <c r="K175" s="27" t="s">
+      <c r="L175" s="29" t="s">
         <v>885</v>
-      </c>
-      <c r="L175" s="29" t="s">
-        <v>886</v>
       </c>
       <c r="M175" s="28"/>
     </row>
@@ -9192,7 +9187,7 @@
         <v>463</v>
       </c>
       <c r="B176" s="27" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C176" s="27">
         <v>175</v>
@@ -9203,22 +9198,22 @@
         <v>7</v>
       </c>
       <c r="G176" s="29" t="s">
+        <v>886</v>
+      </c>
+      <c r="H176" s="27" t="s">
         <v>887</v>
       </c>
-      <c r="H176" s="27" t="s">
+      <c r="I176" s="27" t="s">
         <v>888</v>
       </c>
-      <c r="I176" s="27" t="s">
+      <c r="J176" s="27" t="s">
         <v>889</v>
       </c>
-      <c r="J176" s="27" t="s">
+      <c r="K176" s="27" t="s">
         <v>890</v>
       </c>
-      <c r="K176" s="27" t="s">
+      <c r="L176" s="29" t="s">
         <v>891</v>
-      </c>
-      <c r="L176" s="29" t="s">
-        <v>892</v>
       </c>
       <c r="M176" s="28"/>
     </row>
@@ -9227,7 +9222,7 @@
         <v>463</v>
       </c>
       <c r="B177" s="27" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C177" s="27">
         <v>176</v>
@@ -9238,22 +9233,22 @@
         <v>7</v>
       </c>
       <c r="G177" s="29" t="s">
+        <v>892</v>
+      </c>
+      <c r="H177" s="27" t="s">
         <v>893</v>
       </c>
-      <c r="H177" s="27" t="s">
+      <c r="I177" s="27" t="s">
         <v>894</v>
       </c>
-      <c r="I177" s="27" t="s">
+      <c r="J177" s="27" t="s">
         <v>895</v>
       </c>
-      <c r="J177" s="27" t="s">
+      <c r="K177" s="27" t="s">
         <v>896</v>
       </c>
-      <c r="K177" s="27" t="s">
+      <c r="L177" s="29" t="s">
         <v>897</v>
-      </c>
-      <c r="L177" s="29" t="s">
-        <v>898</v>
       </c>
       <c r="M177" s="28"/>
     </row>
@@ -9262,7 +9257,7 @@
         <v>463</v>
       </c>
       <c r="B178" s="27" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C178" s="27">
         <v>177</v>
@@ -9273,22 +9268,22 @@
         <v>7</v>
       </c>
       <c r="G178" s="29" t="s">
+        <v>898</v>
+      </c>
+      <c r="H178" s="27" t="s">
         <v>899</v>
       </c>
-      <c r="H178" s="27" t="s">
+      <c r="I178" s="27" t="s">
         <v>900</v>
       </c>
-      <c r="I178" s="27" t="s">
+      <c r="J178" s="27" t="s">
         <v>901</v>
       </c>
-      <c r="J178" s="27" t="s">
+      <c r="K178" s="27" t="s">
         <v>902</v>
       </c>
-      <c r="K178" s="27" t="s">
+      <c r="L178" s="29" t="s">
         <v>903</v>
-      </c>
-      <c r="L178" s="29" t="s">
-        <v>904</v>
       </c>
       <c r="M178" s="28"/>
     </row>
@@ -9297,7 +9292,7 @@
         <v>463</v>
       </c>
       <c r="B179" s="27" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C179" s="27">
         <v>178</v>
@@ -9308,22 +9303,22 @@
         <v>7</v>
       </c>
       <c r="G179" s="29" t="s">
+        <v>904</v>
+      </c>
+      <c r="H179" s="27" t="s">
         <v>905</v>
       </c>
-      <c r="H179" s="27" t="s">
+      <c r="I179" s="27" t="s">
         <v>906</v>
       </c>
-      <c r="I179" s="27" t="s">
+      <c r="J179" s="27" t="s">
         <v>907</v>
       </c>
-      <c r="J179" s="27" t="s">
+      <c r="K179" s="27" t="s">
         <v>908</v>
       </c>
-      <c r="K179" s="27" t="s">
+      <c r="L179" s="29" t="s">
         <v>909</v>
-      </c>
-      <c r="L179" s="29" t="s">
-        <v>910</v>
       </c>
       <c r="M179" s="28"/>
     </row>
@@ -9332,7 +9327,7 @@
         <v>463</v>
       </c>
       <c r="B180" s="27" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C180" s="27">
         <v>179</v>
@@ -9343,22 +9338,22 @@
         <v>7</v>
       </c>
       <c r="G180" s="29" t="s">
+        <v>910</v>
+      </c>
+      <c r="H180" s="27" t="s">
         <v>911</v>
       </c>
-      <c r="H180" s="27" t="s">
+      <c r="I180" s="27" t="s">
         <v>912</v>
       </c>
-      <c r="I180" s="27" t="s">
+      <c r="J180" s="27" t="s">
         <v>913</v>
       </c>
-      <c r="J180" s="27" t="s">
+      <c r="K180" s="27" t="s">
         <v>914</v>
       </c>
-      <c r="K180" s="27" t="s">
+      <c r="L180" s="29" t="s">
         <v>915</v>
-      </c>
-      <c r="L180" s="29" t="s">
-        <v>916</v>
       </c>
       <c r="M180" s="28"/>
     </row>
@@ -9367,7 +9362,7 @@
         <v>463</v>
       </c>
       <c r="B181" s="27" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C181" s="27">
         <v>180</v>
@@ -9378,22 +9373,22 @@
         <v>7</v>
       </c>
       <c r="G181" s="29" t="s">
+        <v>916</v>
+      </c>
+      <c r="H181" s="27" t="s">
         <v>917</v>
       </c>
-      <c r="H181" s="27" t="s">
+      <c r="I181" s="27" t="s">
         <v>918</v>
       </c>
-      <c r="I181" s="27" t="s">
+      <c r="J181" s="27" t="s">
         <v>919</v>
       </c>
-      <c r="J181" s="27" t="s">
+      <c r="K181" s="27" t="s">
         <v>920</v>
       </c>
-      <c r="K181" s="27" t="s">
+      <c r="L181" s="29" t="s">
         <v>921</v>
-      </c>
-      <c r="L181" s="29" t="s">
-        <v>922</v>
       </c>
       <c r="M181" s="28"/>
     </row>
@@ -9402,7 +9397,7 @@
         <v>463</v>
       </c>
       <c r="B182" s="27" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C182" s="27">
         <v>181</v>
@@ -9413,22 +9408,22 @@
         <v>7</v>
       </c>
       <c r="G182" s="29" t="s">
+        <v>922</v>
+      </c>
+      <c r="H182" s="27" t="s">
         <v>923</v>
       </c>
-      <c r="H182" s="27" t="s">
+      <c r="I182" s="27" t="s">
         <v>924</v>
       </c>
-      <c r="I182" s="27" t="s">
+      <c r="J182" s="27" t="s">
         <v>925</v>
       </c>
-      <c r="J182" s="27" t="s">
+      <c r="K182" s="27" t="s">
         <v>926</v>
       </c>
-      <c r="K182" s="27" t="s">
+      <c r="L182" s="29" t="s">
         <v>927</v>
-      </c>
-      <c r="L182" s="29" t="s">
-        <v>928</v>
       </c>
       <c r="M182" s="28"/>
     </row>
@@ -9437,7 +9432,7 @@
         <v>463</v>
       </c>
       <c r="B183" s="27" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C183" s="27">
         <v>182</v>
@@ -9448,22 +9443,22 @@
         <v>7</v>
       </c>
       <c r="G183" s="29" t="s">
+        <v>928</v>
+      </c>
+      <c r="H183" s="27" t="s">
         <v>929</v>
       </c>
-      <c r="H183" s="27" t="s">
+      <c r="I183" s="27" t="s">
         <v>930</v>
       </c>
-      <c r="I183" s="27" t="s">
+      <c r="J183" s="27" t="s">
         <v>931</v>
       </c>
-      <c r="J183" s="27" t="s">
+      <c r="K183" s="27" t="s">
         <v>932</v>
       </c>
-      <c r="K183" s="27" t="s">
+      <c r="L183" s="29" t="s">
         <v>933</v>
-      </c>
-      <c r="L183" s="29" t="s">
-        <v>934</v>
       </c>
       <c r="M183" s="28"/>
     </row>
@@ -9472,7 +9467,7 @@
         <v>463</v>
       </c>
       <c r="B184" s="27" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C184" s="27">
         <v>183</v>
@@ -9483,22 +9478,22 @@
         <v>7</v>
       </c>
       <c r="G184" s="29" t="s">
+        <v>934</v>
+      </c>
+      <c r="H184" s="27" t="s">
         <v>935</v>
       </c>
-      <c r="H184" s="27" t="s">
+      <c r="I184" s="27" t="s">
         <v>936</v>
       </c>
-      <c r="I184" s="27" t="s">
+      <c r="J184" s="27" t="s">
         <v>937</v>
       </c>
-      <c r="J184" s="27" t="s">
+      <c r="K184" s="27" t="s">
         <v>938</v>
       </c>
-      <c r="K184" s="27" t="s">
+      <c r="L184" s="29" t="s">
         <v>939</v>
-      </c>
-      <c r="L184" s="29" t="s">
-        <v>940</v>
       </c>
       <c r="M184" s="28"/>
     </row>
@@ -9507,7 +9502,7 @@
         <v>463</v>
       </c>
       <c r="B185" s="27" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C185" s="27">
         <v>184</v>
@@ -9518,22 +9513,22 @@
         <v>7</v>
       </c>
       <c r="G185" s="29" t="s">
+        <v>940</v>
+      </c>
+      <c r="H185" s="27" t="s">
         <v>941</v>
       </c>
-      <c r="H185" s="27" t="s">
+      <c r="I185" s="27" t="s">
         <v>942</v>
       </c>
-      <c r="I185" s="27" t="s">
+      <c r="J185" s="27" t="s">
         <v>943</v>
       </c>
-      <c r="J185" s="27" t="s">
+      <c r="K185" s="27" t="s">
         <v>944</v>
       </c>
-      <c r="K185" s="27" t="s">
+      <c r="L185" s="29" t="s">
         <v>945</v>
-      </c>
-      <c r="L185" s="29" t="s">
-        <v>946</v>
       </c>
       <c r="M185" s="28"/>
     </row>
@@ -9542,7 +9537,7 @@
         <v>463</v>
       </c>
       <c r="B186" s="27" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C186" s="27">
         <v>185</v>
@@ -9553,22 +9548,22 @@
         <v>7</v>
       </c>
       <c r="G186" s="29" t="s">
+        <v>946</v>
+      </c>
+      <c r="H186" s="27" t="s">
         <v>947</v>
       </c>
-      <c r="H186" s="27" t="s">
+      <c r="I186" s="27" t="s">
         <v>948</v>
       </c>
-      <c r="I186" s="27" t="s">
+      <c r="J186" s="27" t="s">
         <v>949</v>
       </c>
-      <c r="J186" s="27" t="s">
+      <c r="K186" s="27" t="s">
         <v>950</v>
       </c>
-      <c r="K186" s="27" t="s">
+      <c r="L186" s="29" t="s">
         <v>951</v>
-      </c>
-      <c r="L186" s="29" t="s">
-        <v>952</v>
       </c>
       <c r="M186" s="28"/>
     </row>
@@ -9577,7 +9572,7 @@
         <v>463</v>
       </c>
       <c r="B187" s="27" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C187" s="27">
         <v>186</v>
@@ -9588,22 +9583,22 @@
         <v>7</v>
       </c>
       <c r="G187" s="29" t="s">
+        <v>952</v>
+      </c>
+      <c r="H187" s="27" t="s">
         <v>953</v>
       </c>
-      <c r="H187" s="27" t="s">
+      <c r="I187" s="27" t="s">
         <v>954</v>
       </c>
-      <c r="I187" s="27" t="s">
+      <c r="J187" s="27" t="s">
         <v>955</v>
       </c>
-      <c r="J187" s="27" t="s">
+      <c r="K187" s="27" t="s">
         <v>956</v>
       </c>
-      <c r="K187" s="27" t="s">
+      <c r="L187" s="29" t="s">
         <v>957</v>
-      </c>
-      <c r="L187" s="29" t="s">
-        <v>958</v>
       </c>
       <c r="M187" s="28"/>
     </row>
@@ -9612,7 +9607,7 @@
         <v>463</v>
       </c>
       <c r="B188" s="27" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C188" s="27">
         <v>187</v>
@@ -9623,22 +9618,22 @@
         <v>7</v>
       </c>
       <c r="G188" s="29" t="s">
+        <v>958</v>
+      </c>
+      <c r="H188" s="27" t="s">
         <v>959</v>
       </c>
-      <c r="H188" s="27" t="s">
+      <c r="I188" s="27" t="s">
         <v>960</v>
       </c>
-      <c r="I188" s="27" t="s">
+      <c r="J188" s="27" t="s">
         <v>961</v>
       </c>
-      <c r="J188" s="27" t="s">
+      <c r="K188" s="27" t="s">
         <v>962</v>
       </c>
-      <c r="K188" s="27" t="s">
+      <c r="L188" s="29" t="s">
         <v>963</v>
-      </c>
-      <c r="L188" s="29" t="s">
-        <v>964</v>
       </c>
       <c r="M188" s="28"/>
     </row>
@@ -9647,7 +9642,7 @@
         <v>463</v>
       </c>
       <c r="B189" s="27" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C189" s="27">
         <v>188</v>
@@ -9658,22 +9653,22 @@
         <v>7</v>
       </c>
       <c r="G189" s="29" t="s">
+        <v>964</v>
+      </c>
+      <c r="H189" s="27" t="s">
         <v>965</v>
       </c>
-      <c r="H189" s="27" t="s">
+      <c r="I189" s="27" t="s">
         <v>966</v>
       </c>
-      <c r="I189" s="27" t="s">
+      <c r="J189" s="27" t="s">
         <v>967</v>
       </c>
-      <c r="J189" s="27" t="s">
+      <c r="K189" s="27" t="s">
         <v>968</v>
       </c>
-      <c r="K189" s="27" t="s">
+      <c r="L189" s="29" t="s">
         <v>969</v>
-      </c>
-      <c r="L189" s="29" t="s">
-        <v>970</v>
       </c>
       <c r="M189" s="28"/>
     </row>
@@ -9682,7 +9677,7 @@
         <v>463</v>
       </c>
       <c r="B190" s="27" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C190" s="27">
         <v>189</v>
@@ -9693,22 +9688,22 @@
         <v>7</v>
       </c>
       <c r="G190" s="29" t="s">
+        <v>970</v>
+      </c>
+      <c r="H190" s="27" t="s">
         <v>971</v>
       </c>
-      <c r="H190" s="27" t="s">
+      <c r="I190" s="27" t="s">
         <v>972</v>
       </c>
-      <c r="I190" s="27" t="s">
+      <c r="J190" s="27" t="s">
         <v>973</v>
       </c>
-      <c r="J190" s="27" t="s">
+      <c r="K190" s="27" t="s">
         <v>974</v>
       </c>
-      <c r="K190" s="27" t="s">
+      <c r="L190" s="29" t="s">
         <v>975</v>
-      </c>
-      <c r="L190" s="29" t="s">
-        <v>976</v>
       </c>
       <c r="M190" s="28"/>
     </row>
@@ -9717,7 +9712,7 @@
         <v>463</v>
       </c>
       <c r="B191" s="27" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C191" s="27">
         <v>190</v>
@@ -9728,22 +9723,22 @@
         <v>7</v>
       </c>
       <c r="G191" s="29" t="s">
+        <v>976</v>
+      </c>
+      <c r="H191" s="27" t="s">
         <v>977</v>
       </c>
-      <c r="H191" s="27" t="s">
+      <c r="I191" s="27" t="s">
         <v>978</v>
       </c>
-      <c r="I191" s="27" t="s">
+      <c r="J191" s="27" t="s">
         <v>979</v>
       </c>
-      <c r="J191" s="27" t="s">
+      <c r="K191" s="27" t="s">
         <v>980</v>
       </c>
-      <c r="K191" s="27" t="s">
+      <c r="L191" s="29" t="s">
         <v>981</v>
-      </c>
-      <c r="L191" s="29" t="s">
-        <v>982</v>
       </c>
       <c r="M191" s="28"/>
     </row>
@@ -9752,7 +9747,7 @@
         <v>463</v>
       </c>
       <c r="B192" s="27" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C192" s="27">
         <v>191</v>
@@ -9763,22 +9758,22 @@
         <v>7</v>
       </c>
       <c r="G192" s="29" t="s">
+        <v>982</v>
+      </c>
+      <c r="H192" s="27" t="s">
         <v>983</v>
       </c>
-      <c r="H192" s="27" t="s">
+      <c r="I192" s="27" t="s">
         <v>984</v>
       </c>
-      <c r="I192" s="27" t="s">
+      <c r="J192" s="27" t="s">
         <v>985</v>
       </c>
-      <c r="J192" s="27" t="s">
+      <c r="K192" s="27" t="s">
         <v>986</v>
       </c>
-      <c r="K192" s="27" t="s">
+      <c r="L192" s="29" t="s">
         <v>987</v>
-      </c>
-      <c r="L192" s="29" t="s">
-        <v>988</v>
       </c>
       <c r="M192" s="28"/>
     </row>
@@ -9787,7 +9782,7 @@
         <v>463</v>
       </c>
       <c r="B193" s="27" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C193" s="27">
         <v>192</v>
@@ -9798,22 +9793,22 @@
         <v>7</v>
       </c>
       <c r="G193" s="29" t="s">
+        <v>988</v>
+      </c>
+      <c r="H193" s="27" t="s">
         <v>989</v>
       </c>
-      <c r="H193" s="27" t="s">
+      <c r="I193" s="27" t="s">
         <v>990</v>
       </c>
-      <c r="I193" s="27" t="s">
+      <c r="J193" s="27" t="s">
         <v>991</v>
       </c>
-      <c r="J193" s="27" t="s">
+      <c r="K193" s="27" t="s">
         <v>992</v>
       </c>
-      <c r="K193" s="27" t="s">
+      <c r="L193" s="29" t="s">
         <v>993</v>
-      </c>
-      <c r="L193" s="29" t="s">
-        <v>994</v>
       </c>
       <c r="M193" s="28"/>
     </row>
@@ -9822,7 +9817,7 @@
         <v>463</v>
       </c>
       <c r="B194" s="27" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C194" s="27">
         <v>193</v>
@@ -9833,22 +9828,22 @@
         <v>7</v>
       </c>
       <c r="G194" s="29" t="s">
+        <v>994</v>
+      </c>
+      <c r="H194" s="27" t="s">
         <v>995</v>
       </c>
-      <c r="H194" s="27" t="s">
+      <c r="I194" s="27" t="s">
         <v>996</v>
       </c>
-      <c r="I194" s="27" t="s">
+      <c r="J194" s="27" t="s">
         <v>997</v>
       </c>
-      <c r="J194" s="27" t="s">
+      <c r="K194" s="27" t="s">
         <v>998</v>
       </c>
-      <c r="K194" s="27" t="s">
+      <c r="L194" s="29" t="s">
         <v>999</v>
-      </c>
-      <c r="L194" s="29" t="s">
-        <v>1000</v>
       </c>
       <c r="M194" s="28"/>
     </row>
@@ -9857,7 +9852,7 @@
         <v>463</v>
       </c>
       <c r="B195" s="27" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C195" s="27">
         <v>194</v>
@@ -9868,22 +9863,22 @@
         <v>7</v>
       </c>
       <c r="G195" s="29" t="s">
+        <v>1000</v>
+      </c>
+      <c r="H195" s="27" t="s">
         <v>1001</v>
       </c>
-      <c r="H195" s="27" t="s">
+      <c r="I195" s="27" t="s">
         <v>1002</v>
       </c>
-      <c r="I195" s="27" t="s">
+      <c r="J195" s="27" t="s">
         <v>1003</v>
       </c>
-      <c r="J195" s="27" t="s">
+      <c r="K195" s="27" t="s">
         <v>1004</v>
       </c>
-      <c r="K195" s="27" t="s">
+      <c r="L195" s="29" t="s">
         <v>1005</v>
-      </c>
-      <c r="L195" s="29" t="s">
-        <v>1006</v>
       </c>
       <c r="M195" s="28"/>
     </row>
@@ -9892,7 +9887,7 @@
         <v>463</v>
       </c>
       <c r="B196" s="27" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C196" s="27">
         <v>195</v>
@@ -9903,22 +9898,22 @@
         <v>7</v>
       </c>
       <c r="G196" s="29" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H196" s="27" t="s">
         <v>1007</v>
       </c>
-      <c r="H196" s="27" t="s">
+      <c r="I196" s="27" t="s">
         <v>1008</v>
       </c>
-      <c r="I196" s="27" t="s">
+      <c r="J196" s="27" t="s">
         <v>1009</v>
       </c>
-      <c r="J196" s="27" t="s">
+      <c r="K196" s="27" t="s">
         <v>1010</v>
       </c>
-      <c r="K196" s="27" t="s">
+      <c r="L196" s="29" t="s">
         <v>1011</v>
-      </c>
-      <c r="L196" s="29" t="s">
-        <v>1012</v>
       </c>
       <c r="M196" s="28"/>
     </row>
@@ -9927,7 +9922,7 @@
         <v>463</v>
       </c>
       <c r="B197" s="27" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C197" s="27">
         <v>196</v>
@@ -9938,22 +9933,22 @@
         <v>7</v>
       </c>
       <c r="G197" s="29" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H197" s="27" t="s">
         <v>1013</v>
       </c>
-      <c r="H197" s="27" t="s">
+      <c r="I197" s="27" t="s">
         <v>1014</v>
       </c>
-      <c r="I197" s="27" t="s">
+      <c r="J197" s="27" t="s">
         <v>1015</v>
       </c>
-      <c r="J197" s="27" t="s">
+      <c r="K197" s="27" t="s">
         <v>1016</v>
       </c>
-      <c r="K197" s="27" t="s">
+      <c r="L197" s="29" t="s">
         <v>1017</v>
-      </c>
-      <c r="L197" s="29" t="s">
-        <v>1018</v>
       </c>
       <c r="M197" s="28"/>
     </row>
@@ -9962,7 +9957,7 @@
         <v>463</v>
       </c>
       <c r="B198" s="27" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C198" s="27">
         <v>197</v>
@@ -9973,22 +9968,22 @@
         <v>7</v>
       </c>
       <c r="G198" s="29" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H198" s="27" t="s">
         <v>1019</v>
       </c>
-      <c r="H198" s="27" t="s">
+      <c r="I198" s="27" t="s">
         <v>1020</v>
       </c>
-      <c r="I198" s="27" t="s">
+      <c r="J198" s="27" t="s">
         <v>1021</v>
       </c>
-      <c r="J198" s="27" t="s">
+      <c r="K198" s="27" t="s">
         <v>1022</v>
       </c>
-      <c r="K198" s="27" t="s">
+      <c r="L198" s="29" t="s">
         <v>1023</v>
-      </c>
-      <c r="L198" s="29" t="s">
-        <v>1024</v>
       </c>
       <c r="M198" s="28"/>
     </row>
@@ -9997,7 +9992,7 @@
         <v>463</v>
       </c>
       <c r="B199" s="27" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C199" s="27">
         <v>198</v>
@@ -10008,22 +10003,22 @@
         <v>7</v>
       </c>
       <c r="G199" s="29" t="s">
+        <v>1024</v>
+      </c>
+      <c r="H199" s="27" t="s">
         <v>1025</v>
       </c>
-      <c r="H199" s="27" t="s">
+      <c r="I199" s="27" t="s">
         <v>1026</v>
       </c>
-      <c r="I199" s="27" t="s">
+      <c r="J199" s="27" t="s">
         <v>1027</v>
       </c>
-      <c r="J199" s="27" t="s">
+      <c r="K199" s="27" t="s">
         <v>1028</v>
       </c>
-      <c r="K199" s="27" t="s">
+      <c r="L199" s="29" t="s">
         <v>1029</v>
-      </c>
-      <c r="L199" s="29" t="s">
-        <v>1030</v>
       </c>
       <c r="M199" s="28"/>
     </row>
@@ -10032,7 +10027,7 @@
         <v>463</v>
       </c>
       <c r="B200" s="27" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C200" s="27">
         <v>199</v>
@@ -10043,22 +10038,22 @@
         <v>7</v>
       </c>
       <c r="G200" s="29" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H200" s="27" t="s">
         <v>1031</v>
       </c>
-      <c r="H200" s="27" t="s">
+      <c r="I200" s="27" t="s">
         <v>1032</v>
       </c>
-      <c r="I200" s="27" t="s">
+      <c r="J200" s="27" t="s">
         <v>1033</v>
       </c>
-      <c r="J200" s="27" t="s">
+      <c r="K200" s="27" t="s">
         <v>1034</v>
       </c>
-      <c r="K200" s="27" t="s">
+      <c r="L200" s="29" t="s">
         <v>1035</v>
-      </c>
-      <c r="L200" s="29" t="s">
-        <v>1036</v>
       </c>
       <c r="M200" s="28"/>
     </row>
@@ -10067,7 +10062,7 @@
         <v>463</v>
       </c>
       <c r="B201" s="27" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C201" s="27">
         <v>200</v>
@@ -10078,22 +10073,22 @@
         <v>7</v>
       </c>
       <c r="G201" s="29" t="s">
+        <v>1036</v>
+      </c>
+      <c r="H201" s="27" t="s">
         <v>1037</v>
       </c>
-      <c r="H201" s="27" t="s">
+      <c r="I201" s="27" t="s">
         <v>1038</v>
       </c>
-      <c r="I201" s="27" t="s">
+      <c r="J201" s="27" t="s">
         <v>1039</v>
       </c>
-      <c r="J201" s="27" t="s">
+      <c r="K201" s="27" t="s">
         <v>1040</v>
       </c>
-      <c r="K201" s="27" t="s">
+      <c r="L201" s="29" t="s">
         <v>1041</v>
-      </c>
-      <c r="L201" s="29" t="s">
-        <v>1042</v>
       </c>
       <c r="M201" s="28"/>
     </row>

</xml_diff>